<commit_message>
logo plots with means, unsure if math is correct yet
</commit_message>
<xml_diff>
--- a/logo_plot_assets/data/nucleotide/sample_dna_equal.xlsx
+++ b/logo_plot_assets/data/nucleotide/sample_dna_equal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://czbiohub-my.sharepoint.com/personal/olivia_yoo_czbiohub_org/Documents/logo_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivia.yoo/Desktop/code/ortho_seqs/logo_plot_assets/data/nucleotide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{C7B9CE41-AECF-C741-97A2-39237999424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AFD2D65-78A6-7441-B1DA-82F5D7E649D2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D48219-E915-5148-98DF-352B321C81EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="4140" windowWidth="20020" windowHeight="12380" xr2:uid="{6CAFC85A-7830-294E-B7C1-007DF29BB081}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ATTCGATGTC</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>TAGGCCAATG</t>
-  </si>
-  <si>
-    <t>GAATGCATGG</t>
-  </si>
-  <si>
-    <t>ACTAGACTAG</t>
   </si>
 </sst>
 </file>
@@ -416,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D3847A-4917-CA47-A347-99D9FEF062B3}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,16 +461,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>